<commit_message>
More data, and removed some old files
</commit_message>
<xml_diff>
--- a/Excel & CSV Sheets/2019 Data/DailyReports/ToRemoveFile.xlsx
+++ b/Excel & CSV Sheets/2019 Data/DailyReports/ToRemoveFile.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="95">
   <si>
     <t>Accident</t>
   </si>
@@ -175,142 +175,130 @@
     <t>Injuries</t>
   </si>
   <si>
+    <t>No Injuries</t>
+  </si>
+  <si>
     <t>Unknown Injuries</t>
   </si>
   <si>
-    <t>2019-02-05</t>
-  </si>
-  <si>
-    <t>18:51:00</t>
-  </si>
-  <si>
-    <t>16:07:35</t>
-  </si>
-  <si>
-    <t>16:04:22</t>
-  </si>
-  <si>
-    <t>15:37:11</t>
-  </si>
-  <si>
-    <t>15:36:25</t>
-  </si>
-  <si>
-    <t>11:09:07</t>
-  </si>
-  <si>
-    <t>11:08:59</t>
-  </si>
-  <si>
-    <t>09:43:59</t>
-  </si>
-  <si>
-    <t>09:27:05</t>
-  </si>
-  <si>
-    <t>09:25:23</t>
-  </si>
-  <si>
-    <t>08:56:51</t>
-  </si>
-  <si>
-    <t>08:01:18</t>
-  </si>
-  <si>
-    <t>08:01:00</t>
-  </si>
-  <si>
-    <t>07:25:21</t>
-  </si>
-  <si>
-    <t>06:58:47</t>
-  </si>
-  <si>
-    <t>06:57:54</t>
-  </si>
-  <si>
-    <t>06:55:55</t>
-  </si>
-  <si>
-    <t>06:55:14</t>
-  </si>
-  <si>
-    <t>06:54:08</t>
-  </si>
-  <si>
-    <t>06:53:20</t>
-  </si>
-  <si>
-    <t>Hurricane Creek Rd / E Brainerd Rd</t>
-  </si>
-  <si>
-    <t>CUMMINGS HWY / BROWNS FERRY RD</t>
-  </si>
-  <si>
-    <t>3000 CUMMINGS HWY</t>
-  </si>
-  <si>
-    <t>4300-4324 N Access Rd</t>
-  </si>
-  <si>
-    <t>2130 Amnicola Hwy</t>
-  </si>
-  <si>
-    <t>6735 Ringgold Rd</t>
-  </si>
-  <si>
-    <t>400 Palmetto St</t>
-  </si>
-  <si>
-    <t>Dodds Ave / E 24th St</t>
-  </si>
-  <si>
-    <t>1500 Dodds Ave</t>
-  </si>
-  <si>
-    <t>1500 DODDS AVE</t>
-  </si>
-  <si>
-    <t>18000 Interstate 24 Eb</t>
-  </si>
-  <si>
-    <t>San Hsi Dr / Ringgold Rd</t>
-  </si>
-  <si>
-    <t>E Main St / Dodds Ave</t>
-  </si>
-  <si>
-    <t>2600 E MAIN ST</t>
+    <t>2019-02-10</t>
+  </si>
+  <si>
+    <t>21:11:14</t>
+  </si>
+  <si>
+    <t>20:59:19</t>
+  </si>
+  <si>
+    <t>19:40:22</t>
+  </si>
+  <si>
+    <t>19:34:19</t>
+  </si>
+  <si>
+    <t>19:32:33</t>
+  </si>
+  <si>
+    <t>17:47:04</t>
+  </si>
+  <si>
+    <t>17:46:21</t>
+  </si>
+  <si>
+    <t>15:17:13</t>
+  </si>
+  <si>
+    <t>15:16:58</t>
+  </si>
+  <si>
+    <t>14:52:14</t>
+  </si>
+  <si>
+    <t>14:51:45</t>
+  </si>
+  <si>
+    <t>13:31:24</t>
+  </si>
+  <si>
+    <t>13:30:47</t>
+  </si>
+  <si>
+    <t>12:57:25</t>
+  </si>
+  <si>
+    <t>12:14:31</t>
+  </si>
+  <si>
+    <t>10:30:34</t>
+  </si>
+  <si>
+    <t>780 - 899 Glenwood Dr</t>
+  </si>
+  <si>
+    <t>780-898 Glenwood Dr</t>
+  </si>
+  <si>
+    <t>BILL REED RD / GREEN SHANTY RD</t>
+  </si>
+  <si>
+    <t>3871 Hixson Pike</t>
+  </si>
+  <si>
+    <t>Roberts Mill Rd / Hixson Springs Rd</t>
+  </si>
+  <si>
+    <t>18000 Interstate 24 Wb</t>
+  </si>
+  <si>
+    <t>5440 Highway 153</t>
+  </si>
+  <si>
+    <t>Old Dayton Pike / Lynnolen Ln</t>
+  </si>
+  <si>
+    <t>4 LYNNOLEN LN</t>
+  </si>
+  <si>
+    <t>160 INTERSTATE 75 NB</t>
+  </si>
+  <si>
+    <t>9000 Lee Hwy</t>
+  </si>
+  <si>
+    <t>5426 - 5499 School St</t>
   </si>
   <si>
     <t>CHATTANOOGA</t>
   </si>
   <si>
-    <t>EAST RIDGE</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>16</t>
+    <t>HAMILTON COUNTY</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>17</t>
   </si>
   <si>
     <t>15</t>
   </si>
   <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>6</t>
+    <t>14</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>10</t>
   </si>
 </sst>
 </file>
@@ -668,7 +656,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BA24"/>
+  <dimension ref="A1:BA19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -834,31 +822,31 @@
     </row>
     <row r="2" spans="1:53">
       <c r="A2" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
         <v>52</v>
       </c>
       <c r="D2">
-        <v>35.000853</v>
+        <v>35.04172</v>
       </c>
       <c r="E2">
-        <v>-85.132549</v>
+        <v>-85.25831599999999</v>
       </c>
       <c r="F2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="K2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="P2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="Y2">
         <v>2</v>
@@ -866,31 +854,31 @@
     </row>
     <row r="3" spans="1:53">
       <c r="A3" s="1">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
         <v>52</v>
       </c>
       <c r="D3">
-        <v>35.000853</v>
+        <v>35.04212</v>
       </c>
       <c r="E3">
-        <v>-85.132549</v>
+        <v>-85.25808499999999</v>
       </c>
       <c r="F3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K3" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="P3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="Y3">
         <v>2</v>
@@ -898,31 +886,31 @@
     </row>
     <row r="4" spans="1:53">
       <c r="A4" s="1">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D4">
-        <v>35.020313</v>
+        <v>35.045636</v>
       </c>
       <c r="E4">
-        <v>-85.365756</v>
+        <v>-85.110522</v>
       </c>
       <c r="F4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="P4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="Y4">
         <v>2</v>
@@ -930,31 +918,31 @@
     </row>
     <row r="5" spans="1:53">
       <c r="A5" s="1">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
         <v>52</v>
       </c>
       <c r="D5">
-        <v>35.020313</v>
+        <v>35.112743</v>
       </c>
       <c r="E5">
-        <v>-85.365756</v>
+        <v>-85.266201</v>
       </c>
       <c r="F5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K5" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="P5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="Y5">
         <v>2</v>
@@ -962,31 +950,31 @@
     </row>
     <row r="6" spans="1:53">
       <c r="A6" s="1">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
         <v>52</v>
       </c>
       <c r="D6">
-        <v>35.112321</v>
+        <v>35.112743</v>
       </c>
       <c r="E6">
-        <v>-85.252163</v>
+        <v>-85.266201</v>
       </c>
       <c r="F6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="K6" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="P6" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="Y6">
         <v>2</v>
@@ -994,31 +982,31 @@
     </row>
     <row r="7" spans="1:53">
       <c r="A7" s="1">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
         <v>52</v>
       </c>
       <c r="D7">
-        <v>35.112321</v>
+        <v>35.218503</v>
       </c>
       <c r="E7">
-        <v>-85.252163</v>
+        <v>-85.27296800000001</v>
       </c>
       <c r="F7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G7" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K7" t="s">
+        <v>85</v>
+      </c>
+      <c r="P7" t="s">
         <v>89</v>
-      </c>
-      <c r="P7" t="s">
-        <v>93</v>
       </c>
       <c r="Y7">
         <v>2</v>
@@ -1026,31 +1014,31 @@
     </row>
     <row r="8" spans="1:53">
       <c r="A8" s="1">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
         <v>52</v>
       </c>
       <c r="D8">
-        <v>35.065062</v>
+        <v>35.218503</v>
       </c>
       <c r="E8">
-        <v>-85.272718</v>
+        <v>-85.27296800000001</v>
       </c>
       <c r="F8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G8" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P8" t="s">
         <v>89</v>
-      </c>
-      <c r="P8" t="s">
-        <v>94</v>
       </c>
       <c r="Y8">
         <v>2</v>
@@ -1058,31 +1046,31 @@
     </row>
     <row r="9" spans="1:53">
       <c r="A9" s="1">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
         <v>52</v>
       </c>
       <c r="D9">
-        <v>35.065062</v>
+        <v>35.02156</v>
       </c>
       <c r="E9">
-        <v>-85.272718</v>
+        <v>-85.297411</v>
       </c>
       <c r="F9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G9" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K9" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="P9" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="Y9">
         <v>2</v>
@@ -1090,31 +1078,31 @@
     </row>
     <row r="10" spans="1:53">
       <c r="A10" s="1">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D10">
-        <v>34.989228</v>
+        <v>35.02156</v>
       </c>
       <c r="E10">
-        <v>-85.19351899999999</v>
+        <v>-85.297411</v>
       </c>
       <c r="F10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G10" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H10" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="K10" t="s">
+        <v>84</v>
+      </c>
+      <c r="P10" t="s">
         <v>90</v>
-      </c>
-      <c r="P10" t="s">
-        <v>95</v>
       </c>
       <c r="Y10">
         <v>2</v>
@@ -1122,31 +1110,31 @@
     </row>
     <row r="11" spans="1:53">
       <c r="A11" s="1">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C11" t="s">
         <v>52</v>
       </c>
       <c r="D11">
-        <v>35.046723</v>
+        <v>35.138778</v>
       </c>
       <c r="E11">
-        <v>-85.293772</v>
+        <v>-85.24719399999999</v>
       </c>
       <c r="F11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G11" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H11" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K11" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="P11" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="Y11">
         <v>2</v>
@@ -1154,31 +1142,31 @@
     </row>
     <row r="12" spans="1:53">
       <c r="A12" s="1">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
         <v>52</v>
       </c>
       <c r="D12">
-        <v>35.046723</v>
+        <v>35.138778</v>
       </c>
       <c r="E12">
-        <v>-85.293772</v>
+        <v>-85.24719399999999</v>
       </c>
       <c r="F12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G12" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K12" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="P12" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="Y12">
         <v>2</v>
@@ -1186,31 +1174,31 @@
     </row>
     <row r="13" spans="1:53">
       <c r="A13" s="1">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C13" t="s">
         <v>52</v>
       </c>
       <c r="D13">
-        <v>35.01406</v>
+        <v>35.148021</v>
       </c>
       <c r="E13">
-        <v>-85.27455399999999</v>
+        <v>-85.273262</v>
       </c>
       <c r="F13" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G13" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H13" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K13" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="P13" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="Y13">
         <v>2</v>
@@ -1218,31 +1206,31 @@
     </row>
     <row r="14" spans="1:53">
       <c r="A14" s="1">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C14" t="s">
         <v>52</v>
       </c>
       <c r="D14">
-        <v>35.01406</v>
+        <v>35.148035</v>
       </c>
       <c r="E14">
-        <v>-85.27455399999999</v>
+        <v>-85.27331</v>
       </c>
       <c r="F14" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G14" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="H14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="K14" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="P14" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="Y14">
         <v>2</v>
@@ -1253,28 +1241,28 @@
         <v>62</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D15">
-        <v>35.02197</v>
+        <v>35.005828</v>
       </c>
       <c r="E15">
-        <v>-85.26953</v>
+        <v>-85.207205</v>
       </c>
       <c r="F15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G15" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="H15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K15" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="P15" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="Y15">
         <v>2</v>
@@ -1282,31 +1270,31 @@
     </row>
     <row r="16" spans="1:53">
       <c r="A16" s="1">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C16" t="s">
         <v>53</v>
       </c>
       <c r="D16">
-        <v>35.022043</v>
+        <v>35.085686</v>
       </c>
       <c r="E16">
-        <v>-85.269408</v>
+        <v>-85.066688</v>
       </c>
       <c r="F16" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G16" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="H16" t="s">
+        <v>82</v>
+      </c>
+      <c r="K16" t="s">
         <v>84</v>
       </c>
-      <c r="K16" t="s">
-        <v>89</v>
-      </c>
       <c r="P16" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="Y16">
         <v>2</v>
@@ -1314,31 +1302,31 @@
     </row>
     <row r="17" spans="1:25">
       <c r="A17" s="1">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C17" t="s">
         <v>52</v>
       </c>
       <c r="D17">
-        <v>35.021809</v>
+        <v>35.071818</v>
       </c>
       <c r="E17">
-        <v>-85.297892</v>
+        <v>-85.101742</v>
       </c>
       <c r="F17" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G17" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="H17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K17" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="P17" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="Y17">
         <v>2</v>
@@ -1346,31 +1334,31 @@
     </row>
     <row r="18" spans="1:25">
       <c r="A18" s="1">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C18" t="s">
         <v>52</v>
       </c>
       <c r="D18">
-        <v>34.990498</v>
+        <v>35.071818</v>
       </c>
       <c r="E18">
-        <v>-85.22026200000001</v>
+        <v>-85.101742</v>
       </c>
       <c r="F18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G18" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H18" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="K18" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="P18" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="Y18">
         <v>2</v>
@@ -1378,193 +1366,33 @@
     </row>
     <row r="19" spans="1:25">
       <c r="A19" s="1">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C19" t="s">
         <v>52</v>
       </c>
       <c r="D19">
-        <v>34.990498</v>
+        <v>35.071818</v>
       </c>
       <c r="E19">
-        <v>-85.22026200000001</v>
+        <v>-85.101742</v>
       </c>
       <c r="F19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G19" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H19" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="K19" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="P19" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="Y19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:25">
-      <c r="A20" s="1">
-        <v>79</v>
-      </c>
-      <c r="C20" t="s">
-        <v>52</v>
-      </c>
-      <c r="D20">
-        <v>35.022196</v>
-      </c>
-      <c r="E20">
-        <v>-85.269492</v>
-      </c>
-      <c r="F20" t="s">
-        <v>54</v>
-      </c>
-      <c r="G20" t="s">
-        <v>71</v>
-      </c>
-      <c r="H20" t="s">
-        <v>87</v>
-      </c>
-      <c r="K20" t="s">
-        <v>89</v>
-      </c>
-      <c r="P20" t="s">
-        <v>98</v>
-      </c>
-      <c r="Y20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:25">
-      <c r="A21" s="1">
-        <v>80</v>
-      </c>
-      <c r="C21" t="s">
-        <v>52</v>
-      </c>
-      <c r="D21">
-        <v>35.022196</v>
-      </c>
-      <c r="E21">
-        <v>-85.269492</v>
-      </c>
-      <c r="F21" t="s">
-        <v>54</v>
-      </c>
-      <c r="G21" t="s">
-        <v>72</v>
-      </c>
-      <c r="H21" t="s">
-        <v>87</v>
-      </c>
-      <c r="K21" t="s">
-        <v>89</v>
-      </c>
-      <c r="P21" t="s">
-        <v>98</v>
-      </c>
-      <c r="Y21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:25">
-      <c r="A22" s="1">
-        <v>81</v>
-      </c>
-      <c r="C22" t="s">
-        <v>52</v>
-      </c>
-      <c r="D22">
-        <v>35.022196</v>
-      </c>
-      <c r="E22">
-        <v>-85.269492</v>
-      </c>
-      <c r="F22" t="s">
-        <v>54</v>
-      </c>
-      <c r="G22" t="s">
-        <v>73</v>
-      </c>
-      <c r="H22" t="s">
-        <v>87</v>
-      </c>
-      <c r="K22" t="s">
-        <v>89</v>
-      </c>
-      <c r="P22" t="s">
-        <v>98</v>
-      </c>
-      <c r="Y22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:25">
-      <c r="A23" s="1">
-        <v>82</v>
-      </c>
-      <c r="C23" t="s">
-        <v>52</v>
-      </c>
-      <c r="D23">
-        <v>35.022196</v>
-      </c>
-      <c r="E23">
-        <v>-85.269492</v>
-      </c>
-      <c r="F23" t="s">
-        <v>54</v>
-      </c>
-      <c r="G23" t="s">
-        <v>73</v>
-      </c>
-      <c r="H23" t="s">
-        <v>87</v>
-      </c>
-      <c r="K23" t="s">
-        <v>89</v>
-      </c>
-      <c r="P23" t="s">
-        <v>98</v>
-      </c>
-      <c r="Y23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:25">
-      <c r="A24" s="1">
-        <v>83</v>
-      </c>
-      <c r="C24" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24">
-        <v>35.022196</v>
-      </c>
-      <c r="E24">
-        <v>-85.269492</v>
-      </c>
-      <c r="F24" t="s">
-        <v>54</v>
-      </c>
-      <c r="G24" t="s">
-        <v>74</v>
-      </c>
-      <c r="H24" t="s">
-        <v>88</v>
-      </c>
-      <c r="K24" t="s">
-        <v>89</v>
-      </c>
-      <c r="P24" t="s">
-        <v>98</v>
-      </c>
-      <c r="Y24">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
This is the first push from the laptop, hopefully it works
</commit_message>
<xml_diff>
--- a/Excel & CSV Sheets/2019 Data/DailyReports/ToRemoveFile.xlsx
+++ b/Excel & CSV Sheets/2019 Data/DailyReports/ToRemoveFile.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="90">
   <si>
     <t>Accident</t>
   </si>
@@ -61,9 +61,6 @@
     <t>Hour</t>
   </si>
   <si>
-    <t>Unix</t>
-  </si>
-  <si>
     <t>Temperature</t>
   </si>
   <si>
@@ -178,121 +175,94 @@
     <t>Injuries</t>
   </si>
   <si>
-    <t>Mass Casualty</t>
-  </si>
-  <si>
     <t>Unknown Injuries</t>
   </si>
   <si>
     <t>No Injuries</t>
   </si>
   <si>
-    <t>2019-03-26</t>
-  </si>
-  <si>
-    <t>21:32:57</t>
-  </si>
-  <si>
-    <t>21:23:55</t>
-  </si>
-  <si>
-    <t>21:23:46</t>
-  </si>
-  <si>
-    <t>18:29:42</t>
-  </si>
-  <si>
-    <t>18:28:40</t>
-  </si>
-  <si>
-    <t>18:28:23</t>
-  </si>
-  <si>
-    <t>18:28:21</t>
-  </si>
-  <si>
-    <t>17:52:09</t>
-  </si>
-  <si>
-    <t>17:50:02</t>
-  </si>
-  <si>
-    <t>17:49:52</t>
-  </si>
-  <si>
-    <t>17:00:12</t>
-  </si>
-  <si>
-    <t>14:40:47</t>
-  </si>
-  <si>
-    <t>14:08:08</t>
-  </si>
-  <si>
-    <t>14:07:50</t>
-  </si>
-  <si>
-    <t>10:20:36</t>
-  </si>
-  <si>
-    <t>10:19:45</t>
-  </si>
-  <si>
-    <t>06:10:22</t>
-  </si>
-  <si>
-    <t>3204 Brainerd Rd</t>
-  </si>
-  <si>
-    <t>796 Ridgeway Ave</t>
-  </si>
-  <si>
-    <t>6000 - 6199 Mountain View Rd</t>
-  </si>
-  <si>
-    <t>5728 HIGHWAY 58</t>
-  </si>
-  <si>
-    <t>5728 Highway 58</t>
-  </si>
-  <si>
-    <t>4900-4922 Brainerd Rd</t>
-  </si>
-  <si>
-    <t>3820 Granada Dr</t>
-  </si>
-  <si>
-    <t>Brainerd Rd / Belvoir Ave</t>
-  </si>
-  <si>
-    <t>1-9 Exit Dayton Pike On Ramp Sb</t>
-  </si>
-  <si>
-    <t>5900 Pine Grove Trl</t>
-  </si>
-  <si>
-    <t>8900-8989 Highway 58</t>
-  </si>
-  <si>
-    <t>11-19 Exit 4a Off Ramp Nb</t>
-  </si>
-  <si>
-    <t>1 N MOORE RD</t>
+    <t>Entrapment</t>
+  </si>
+  <si>
+    <t>2019-04-03</t>
+  </si>
+  <si>
+    <t>20:35:10</t>
+  </si>
+  <si>
+    <t>19:16:39</t>
+  </si>
+  <si>
+    <t>18:42:28</t>
+  </si>
+  <si>
+    <t>17:15:36</t>
+  </si>
+  <si>
+    <t>16:49:12</t>
+  </si>
+  <si>
+    <t>15:53:38</t>
+  </si>
+  <si>
+    <t>15:50:20</t>
+  </si>
+  <si>
+    <t>15:48:49</t>
+  </si>
+  <si>
+    <t>11:16:41</t>
+  </si>
+  <si>
+    <t>09:57:53</t>
+  </si>
+  <si>
+    <t>00:58:39</t>
+  </si>
+  <si>
+    <t>6309 - 6399 Highway 58</t>
+  </si>
+  <si>
+    <t>6404 - 6509 Hixson Pike</t>
+  </si>
+  <si>
+    <t>5300-5315 Ringgold Rd</t>
+  </si>
+  <si>
+    <t>2-8 Exit 4a On Ramp Sb</t>
+  </si>
+  <si>
+    <t>7735 MAGGIE LN</t>
+  </si>
+  <si>
+    <t>500-506 S Germantown Rd</t>
+  </si>
+  <si>
+    <t>N Terrace / S Germantown Rd</t>
+  </si>
+  <si>
+    <t>300 E Martin Luther King Blvd</t>
+  </si>
+  <si>
+    <t>1900 Market St</t>
+  </si>
+  <si>
+    <t>7035 Highway 153</t>
+  </si>
+  <si>
+    <t>HAMILTON COUNTY</t>
   </si>
   <si>
     <t>CHATTANOOGA</t>
   </si>
   <si>
-    <t>SIGNAL MOUNTAIN</t>
-  </si>
-  <si>
-    <t>SODDY DAISY</t>
-  </si>
-  <si>
-    <t>HAMILTON COUNTY</t>
-  </si>
-  <si>
-    <t>21</t>
+    <t>EAST RIDGE</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>19</t>
   </si>
   <si>
     <t>18</t>
@@ -301,13 +271,19 @@
     <t>17</t>
   </si>
   <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>6</t>
+    <t>16</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
 </sst>
 </file>
@@ -665,13 +641,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BB20"/>
+  <dimension ref="A1:BA13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:54">
+    <row r="1" spans="1:53">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -828,616 +804,389 @@
       <c r="BA1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="BB1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:53">
+      <c r="A2" s="1">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="2" spans="1:54">
-      <c r="A2" s="1">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>53</v>
-      </c>
       <c r="D2">
-        <v>35.027325</v>
+        <v>35.124503</v>
       </c>
       <c r="E2">
-        <v>-85.25477600000001</v>
+        <v>-85.125298</v>
       </c>
       <c r="F2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" t="s">
         <v>57</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K2" t="s">
+        <v>78</v>
+      </c>
+      <c r="P2" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:53">
+      <c r="A3" s="1">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3">
+        <v>35.159409</v>
+      </c>
+      <c r="E3">
+        <v>-85.193929</v>
+      </c>
+      <c r="F3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" t="s">
         <v>58</v>
       </c>
-      <c r="H2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K2" t="s">
-        <v>88</v>
-      </c>
-      <c r="P2" t="s">
-        <v>92</v>
-      </c>
-      <c r="Z2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:54">
-      <c r="A3" s="1">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D3">
-        <v>35.121962</v>
-      </c>
-      <c r="E3">
-        <v>-85.343452</v>
-      </c>
-      <c r="F3" t="s">
-        <v>57</v>
-      </c>
-      <c r="G3" t="s">
-        <v>59</v>
-      </c>
       <c r="H3" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="K3" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="P3" t="s">
-        <v>92</v>
-      </c>
-      <c r="Z3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:54">
+        <v>82</v>
+      </c>
+      <c r="Y3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:53">
       <c r="A4" s="1">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
         <v>53</v>
       </c>
       <c r="D4">
-        <v>35.087998</v>
+        <v>34.995118</v>
       </c>
       <c r="E4">
-        <v>-85.065022</v>
+        <v>-85.23435000000001</v>
       </c>
       <c r="F4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H4" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="K4" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="P4" t="s">
-        <v>92</v>
-      </c>
-      <c r="Z4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:54">
+        <v>83</v>
+      </c>
+      <c r="Y4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:53">
       <c r="A5" s="1">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D5">
-        <v>35.087998</v>
+        <v>35.0356</v>
       </c>
       <c r="E5">
-        <v>-85.065022</v>
+        <v>-85.16376</v>
       </c>
       <c r="F5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G5" t="s">
         <v>60</v>
       </c>
       <c r="H5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="K5" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="P5" t="s">
-        <v>92</v>
-      </c>
-      <c r="Z5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:54">
+        <v>84</v>
+      </c>
+      <c r="Y5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:53">
       <c r="A6" s="1">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D6">
-        <v>35.109673</v>
+        <v>35.276261</v>
       </c>
       <c r="E6">
-        <v>-85.13543</v>
+        <v>-84.986068</v>
       </c>
       <c r="F6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G6" t="s">
         <v>61</v>
       </c>
       <c r="H6" t="s">
+        <v>72</v>
+      </c>
+      <c r="K6" t="s">
         <v>78</v>
       </c>
-      <c r="K6" t="s">
-        <v>88</v>
-      </c>
       <c r="P6" t="s">
-        <v>93</v>
-      </c>
-      <c r="Z6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:54">
+        <v>85</v>
+      </c>
+      <c r="Y6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:53">
       <c r="A7" s="1">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D7">
-        <v>35.109673</v>
+        <v>35.01475</v>
       </c>
       <c r="E7">
-        <v>-85.13543</v>
+        <v>-85.2516</v>
       </c>
       <c r="F7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G7" t="s">
         <v>62</v>
       </c>
       <c r="H7" t="s">
+        <v>73</v>
+      </c>
+      <c r="K7" t="s">
         <v>79</v>
       </c>
-      <c r="K7" t="s">
-        <v>88</v>
-      </c>
       <c r="P7" t="s">
-        <v>93</v>
-      </c>
-      <c r="Z7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:54">
+        <v>86</v>
+      </c>
+      <c r="Y7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:53">
       <c r="A8" s="1">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D8">
-        <v>35.109673</v>
+        <v>35.014733</v>
       </c>
       <c r="E8">
-        <v>-85.13543</v>
+        <v>-85.251611</v>
       </c>
       <c r="F8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H8" t="s">
+        <v>74</v>
+      </c>
+      <c r="K8" t="s">
         <v>79</v>
       </c>
-      <c r="K8" t="s">
-        <v>88</v>
-      </c>
       <c r="P8" t="s">
-        <v>93</v>
-      </c>
-      <c r="Z8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:54">
+        <v>86</v>
+      </c>
+      <c r="Y8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:53">
       <c r="A9" s="1">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D9">
-        <v>35.109673</v>
+        <v>35.014733</v>
       </c>
       <c r="E9">
-        <v>-85.13543</v>
+        <v>-85.251611</v>
       </c>
       <c r="F9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H9" t="s">
+        <v>74</v>
+      </c>
+      <c r="K9" t="s">
         <v>79</v>
       </c>
-      <c r="K9" t="s">
-        <v>88</v>
-      </c>
       <c r="P9" t="s">
-        <v>93</v>
-      </c>
-      <c r="Z9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:54">
+        <v>86</v>
+      </c>
+      <c r="Y9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:53">
       <c r="A10" s="1">
-        <v>22</v>
+        <v>82</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D10">
-        <v>35.109673</v>
+        <v>35.044307</v>
       </c>
       <c r="E10">
-        <v>-85.13543</v>
+        <v>-85.305353</v>
       </c>
       <c r="F10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H10" t="s">
+        <v>75</v>
+      </c>
+      <c r="K10" t="s">
         <v>79</v>
       </c>
-      <c r="K10" t="s">
-        <v>88</v>
-      </c>
       <c r="P10" t="s">
-        <v>93</v>
-      </c>
-      <c r="Z10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:54">
+        <v>87</v>
+      </c>
+      <c r="Y10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:53">
       <c r="A11" s="1">
-        <v>32</v>
+        <v>83</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D11">
-        <v>35.01247</v>
+        <v>35.044307</v>
       </c>
       <c r="E11">
-        <v>-85.2272</v>
+        <v>-85.305353</v>
       </c>
       <c r="F11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G11" t="s">
         <v>65</v>
       </c>
       <c r="H11" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="K11" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="P11" t="s">
-        <v>94</v>
-      </c>
-      <c r="Z11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:54">
+        <v>87</v>
+      </c>
+      <c r="Y11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:53">
       <c r="A12" s="1">
-        <v>35</v>
+        <v>92</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D12">
-        <v>35.01985</v>
+        <v>35.032085</v>
       </c>
       <c r="E12">
-        <v>-85.241469</v>
+        <v>-85.3082</v>
       </c>
       <c r="F12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G12" t="s">
         <v>66</v>
       </c>
       <c r="H12" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="K12" t="s">
+        <v>79</v>
+      </c>
+      <c r="P12" t="s">
         <v>88</v>
       </c>
-      <c r="P12" t="s">
-        <v>94</v>
-      </c>
-      <c r="Z12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:54">
+      <c r="Y12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:53">
       <c r="A13" s="1">
-        <v>37</v>
+        <v>110</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D13">
-        <v>35.018698</v>
+        <v>35.185629</v>
       </c>
       <c r="E13">
-        <v>-85.239705</v>
+        <v>-85.246926</v>
       </c>
       <c r="F13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G13" t="s">
         <v>67</v>
       </c>
       <c r="H13" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="K13" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="P13" t="s">
-        <v>94</v>
-      </c>
-      <c r="Z13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:54">
-      <c r="A14" s="1">
-        <v>49</v>
-      </c>
-      <c r="C14" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14">
-        <v>35.30013</v>
-      </c>
-      <c r="E14">
-        <v>-85.15161500000001</v>
-      </c>
-      <c r="F14" t="s">
-        <v>57</v>
-      </c>
-      <c r="G14" t="s">
-        <v>68</v>
-      </c>
-      <c r="H14" t="s">
-        <v>83</v>
-      </c>
-      <c r="K14" t="s">
-        <v>90</v>
-      </c>
-      <c r="P14" t="s">
-        <v>94</v>
-      </c>
-      <c r="Z14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:54">
-      <c r="A15" s="1">
-        <v>72</v>
-      </c>
-      <c r="C15" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15">
-        <v>35.023767</v>
-      </c>
-      <c r="E15">
-        <v>-85.20226</v>
-      </c>
-      <c r="F15" t="s">
-        <v>57</v>
-      </c>
-      <c r="G15" t="s">
-        <v>69</v>
-      </c>
-      <c r="H15" t="s">
-        <v>84</v>
-      </c>
-      <c r="K15" t="s">
-        <v>88</v>
-      </c>
-      <c r="P15" t="s">
-        <v>95</v>
-      </c>
-      <c r="Z15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:54">
-      <c r="A16" s="1">
-        <v>75</v>
-      </c>
-      <c r="C16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D16">
-        <v>35.180718</v>
-      </c>
-      <c r="E16">
-        <v>-85.067359</v>
-      </c>
-      <c r="F16" t="s">
-        <v>57</v>
-      </c>
-      <c r="G16" t="s">
-        <v>70</v>
-      </c>
-      <c r="H16" t="s">
-        <v>85</v>
-      </c>
-      <c r="K16" t="s">
-        <v>91</v>
-      </c>
-      <c r="P16" t="s">
-        <v>95</v>
-      </c>
-      <c r="Z16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:26">
-      <c r="A17" s="1">
-        <v>76</v>
-      </c>
-      <c r="C17" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17">
-        <v>35.180718</v>
-      </c>
-      <c r="E17">
-        <v>-85.067359</v>
-      </c>
-      <c r="F17" t="s">
-        <v>57</v>
-      </c>
-      <c r="G17" t="s">
-        <v>71</v>
-      </c>
-      <c r="H17" t="s">
-        <v>85</v>
-      </c>
-      <c r="K17" t="s">
-        <v>91</v>
-      </c>
-      <c r="P17" t="s">
-        <v>95</v>
-      </c>
-      <c r="Z17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:26">
-      <c r="A18" s="1">
-        <v>95</v>
-      </c>
-      <c r="C18" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18">
-        <v>35.03142</v>
-      </c>
-      <c r="E18">
-        <v>-85.16741</v>
-      </c>
-      <c r="F18" t="s">
-        <v>57</v>
-      </c>
-      <c r="G18" t="s">
-        <v>72</v>
-      </c>
-      <c r="H18" t="s">
-        <v>86</v>
-      </c>
-      <c r="K18" t="s">
-        <v>88</v>
-      </c>
-      <c r="P18" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:26">
-      <c r="A19" s="1">
-        <v>96</v>
-      </c>
-      <c r="C19" t="s">
-        <v>56</v>
-      </c>
-      <c r="D19">
-        <v>35.03142</v>
-      </c>
-      <c r="E19">
-        <v>-85.16741</v>
-      </c>
-      <c r="F19" t="s">
-        <v>57</v>
-      </c>
-      <c r="G19" t="s">
-        <v>73</v>
-      </c>
-      <c r="H19" t="s">
-        <v>86</v>
-      </c>
-      <c r="K19" t="s">
-        <v>88</v>
-      </c>
-      <c r="P19" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:26">
-      <c r="A20" s="1">
-        <v>107</v>
-      </c>
-      <c r="C20" t="s">
-        <v>55</v>
-      </c>
-      <c r="D20">
-        <v>35.012954</v>
-      </c>
-      <c r="E20">
-        <v>-85.22827700000001</v>
-      </c>
-      <c r="F20" t="s">
-        <v>57</v>
-      </c>
-      <c r="G20" t="s">
-        <v>74</v>
-      </c>
-      <c r="H20" t="s">
-        <v>87</v>
-      </c>
-      <c r="K20" t="s">
-        <v>88</v>
-      </c>
-      <c r="P20" t="s">
-        <v>97</v>
-      </c>
-      <c r="Z20">
-        <v>3</v>
+        <v>89</v>
+      </c>
+      <c r="Y13">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Data added for catching up with data collection after spring semester
</commit_message>
<xml_diff>
--- a/Excel & CSV Sheets/2019 Data/DailyReports/ToRemoveFile.xlsx
+++ b/Excel & CSV Sheets/2019 Data/DailyReports/ToRemoveFile.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="105">
   <si>
     <t>Accident</t>
   </si>
@@ -178,153 +178,141 @@
     <t>No Injuries</t>
   </si>
   <si>
-    <t>Entrapment</t>
-  </si>
-  <si>
-    <t>Unknown Injuries</t>
-  </si>
-  <si>
-    <t>2019-04-05</t>
-  </si>
-  <si>
-    <t>22:37:47</t>
-  </si>
-  <si>
-    <t>18:55:45</t>
-  </si>
-  <si>
-    <t>18:02:35</t>
-  </si>
-  <si>
-    <t>17:52:06</t>
-  </si>
-  <si>
-    <t>17:02:03</t>
-  </si>
-  <si>
-    <t>16:30:24</t>
-  </si>
-  <si>
-    <t>15:55:26</t>
-  </si>
-  <si>
-    <t>15:53:51</t>
-  </si>
-  <si>
-    <t>15:36:16</t>
-  </si>
-  <si>
-    <t>12:40:50</t>
-  </si>
-  <si>
-    <t>12:40:17</t>
-  </si>
-  <si>
-    <t>10:35:03</t>
-  </si>
-  <si>
-    <t>10:08:14</t>
-  </si>
-  <si>
-    <t>09:19:31</t>
-  </si>
-  <si>
-    <t>09:18:56</t>
-  </si>
-  <si>
-    <t>09:18:47</t>
-  </si>
-  <si>
-    <t>08:33:44</t>
-  </si>
-  <si>
-    <t>08:25:52</t>
-  </si>
-  <si>
-    <t>08:25:25</t>
-  </si>
-  <si>
-    <t>08:24:52</t>
-  </si>
-  <si>
-    <t>07:45:46</t>
-  </si>
-  <si>
-    <t>06:55:01</t>
-  </si>
-  <si>
-    <t>4260-4268 Bonny Oaks Dr</t>
-  </si>
-  <si>
-    <t>6400-6599 Highway 58</t>
-  </si>
-  <si>
-    <t>340 Interstate 75 Sb</t>
-  </si>
-  <si>
-    <t>936-1098 Mountain Creek Rd</t>
-  </si>
-  <si>
-    <t>Milne St / Dodson Ave</t>
-  </si>
-  <si>
-    <t>4355 Highway 58</t>
-  </si>
-  <si>
-    <t>12300-12598 Dayton Pike</t>
-  </si>
-  <si>
-    <t>5200 - 5301 Hixson Pike</t>
-  </si>
-  <si>
-    <t>3300 Dodds Ave</t>
-  </si>
-  <si>
-    <t>309 E Main St</t>
-  </si>
-  <si>
-    <t>7300 Shallowford Rd</t>
-  </si>
-  <si>
-    <t>100 Interstate 75 Nb</t>
-  </si>
-  <si>
-    <t>304 - 401 Browns Ferry Rd</t>
-  </si>
-  <si>
-    <t>100 BROWNS FERRY RD</t>
-  </si>
-  <si>
-    <t>70 INTERSTATE 75 NB</t>
-  </si>
-  <si>
-    <t>310 - 349 Highway 153 Sb</t>
-  </si>
-  <si>
-    <t>8010 - 8979 Volkswagen Dr</t>
-  </si>
-  <si>
-    <t>18300 INTERSTATE 24 EB</t>
+    <t>2019-04-22</t>
+  </si>
+  <si>
+    <t>22:53:11</t>
+  </si>
+  <si>
+    <t>22:50:51</t>
+  </si>
+  <si>
+    <t>17:13:06</t>
+  </si>
+  <si>
+    <t>17:11:50</t>
+  </si>
+  <si>
+    <t>17:11:00</t>
+  </si>
+  <si>
+    <t>16:58:12</t>
+  </si>
+  <si>
+    <t>16:57:32</t>
+  </si>
+  <si>
+    <t>16:57:24</t>
+  </si>
+  <si>
+    <t>16:55:49</t>
+  </si>
+  <si>
+    <t>16:37:15</t>
+  </si>
+  <si>
+    <t>16:36:38</t>
+  </si>
+  <si>
+    <t>15:25:05</t>
+  </si>
+  <si>
+    <t>15:09:10</t>
+  </si>
+  <si>
+    <t>14:50:08</t>
+  </si>
+  <si>
+    <t>14:45:03</t>
+  </si>
+  <si>
+    <t>12:22:34</t>
+  </si>
+  <si>
+    <t>10:46:44</t>
+  </si>
+  <si>
+    <t>10:23:33</t>
+  </si>
+  <si>
+    <t>10:17:58</t>
+  </si>
+  <si>
+    <t>10:17:44</t>
+  </si>
+  <si>
+    <t>7105 Middle Valley Rd</t>
+  </si>
+  <si>
+    <t>7105 MIDDLE VALLEY RD</t>
+  </si>
+  <si>
+    <t>S Seminole Dr / Ringgold Rd</t>
+  </si>
+  <si>
+    <t>1010 Lee Pike</t>
+  </si>
+  <si>
+    <t>Ooltewah Georgetown Rd / Lee Hwy</t>
+  </si>
+  <si>
+    <t>OOLTEWAH GEORGETOWN RD / LEE HWY</t>
+  </si>
+  <si>
+    <t>18100 Interstate 24 Eb</t>
+  </si>
+  <si>
+    <t>18120 INTERSTATE 24 EB</t>
+  </si>
+  <si>
+    <t>7200 Shallowford Rd</t>
+  </si>
+  <si>
+    <t>CENTRAL AVE / WORKMAN RD</t>
+  </si>
+  <si>
+    <t>Apison Pike / Old Lee Hwy</t>
+  </si>
+  <si>
+    <t>1527-1679 Highway 27 Sb</t>
+  </si>
+  <si>
+    <t>1310 Highway 27 Sb</t>
+  </si>
+  <si>
+    <t>1 - 9 Exit 11 E On Ramp Sb</t>
+  </si>
+  <si>
+    <t>1619 Gunbarrel Rd</t>
+  </si>
+  <si>
+    <t>248 Northgate Mall Dr</t>
+  </si>
+  <si>
+    <t>4800-4899 Brainerd Rd</t>
+  </si>
+  <si>
+    <t>4823 Brainerd Rd</t>
+  </si>
+  <si>
+    <t>HAMILTON COUNTY</t>
+  </si>
+  <si>
+    <t>EAST RIDGE</t>
+  </si>
+  <si>
+    <t>COLLEGEDALE</t>
   </si>
   <si>
     <t>CHATTANOOGA</t>
   </si>
   <si>
-    <t>HAMILTON COUNTY</t>
-  </si>
-  <si>
     <t>SODDY DAISY</t>
   </si>
   <si>
-    <t>EAST RIDGE</t>
-  </si>
-  <si>
     <t>22</t>
   </si>
   <si>
-    <t>18</t>
-  </si>
-  <si>
     <t>17</t>
   </si>
   <si>
@@ -334,22 +322,13 @@
     <t>15</t>
   </si>
   <si>
+    <t>14</t>
+  </si>
+  <si>
     <t>12</t>
   </si>
   <si>
     <t>10</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>6</t>
   </si>
 </sst>
 </file>
@@ -707,7 +686,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BA24"/>
+  <dimension ref="A1:BA23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -873,31 +852,31 @@
     </row>
     <row r="2" spans="1:53">
       <c r="A2" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>52</v>
       </c>
       <c r="D2">
-        <v>35.080702</v>
+        <v>35.178017</v>
       </c>
       <c r="E2">
-        <v>-85.21418</v>
+        <v>-85.201325</v>
       </c>
       <c r="F2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="K2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="P2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="Y2">
         <v>4</v>
@@ -905,31 +884,31 @@
     </row>
     <row r="3" spans="1:53">
       <c r="A3" s="1">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
         <v>52</v>
       </c>
       <c r="D3">
-        <v>35.131219</v>
+        <v>35.178017</v>
       </c>
       <c r="E3">
-        <v>-85.122823</v>
+        <v>-85.201325</v>
       </c>
       <c r="F3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" t="s">
         <v>56</v>
       </c>
-      <c r="G3" t="s">
-        <v>58</v>
-      </c>
       <c r="H3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="K3" t="s">
+        <v>93</v>
+      </c>
+      <c r="P3" t="s">
         <v>98</v>
-      </c>
-      <c r="P3" t="s">
-        <v>102</v>
       </c>
       <c r="Y3">
         <v>4</v>
@@ -937,31 +916,31 @@
     </row>
     <row r="4" spans="1:53">
       <c r="A4" s="1">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D4">
-        <v>35.016659</v>
+        <v>35.00825</v>
       </c>
       <c r="E4">
-        <v>-85.179377</v>
+        <v>-85.26548</v>
       </c>
       <c r="F4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="K4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="P4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="Y4">
         <v>4</v>
@@ -969,31 +948,31 @@
     </row>
     <row r="5" spans="1:53">
       <c r="A5" s="1">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
         <v>52</v>
       </c>
       <c r="D5">
-        <v>35.10786</v>
+        <v>35.310366</v>
       </c>
       <c r="E5">
-        <v>-85.32541000000001</v>
+        <v>-85.11517600000001</v>
       </c>
       <c r="F5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="K5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="P5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="Y5">
         <v>4</v>
@@ -1001,31 +980,31 @@
     </row>
     <row r="6" spans="1:53">
       <c r="A6" s="1">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
         <v>52</v>
       </c>
       <c r="D6">
-        <v>35.046324</v>
+        <v>35.082749</v>
       </c>
       <c r="E6">
-        <v>-85.26336000000001</v>
+        <v>-85.05853999999999</v>
       </c>
       <c r="F6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="K6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="P6" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="Y6">
         <v>4</v>
@@ -1033,31 +1012,31 @@
     </row>
     <row r="7" spans="1:53">
       <c r="A7" s="1">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
         <v>52</v>
       </c>
       <c r="D7">
-        <v>35.084696</v>
+        <v>35.082749</v>
       </c>
       <c r="E7">
-        <v>-85.203333</v>
+        <v>-85.05853999999999</v>
       </c>
       <c r="F7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H7" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="K7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="P7" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="Y7">
         <v>4</v>
@@ -1065,31 +1044,31 @@
     </row>
     <row r="8" spans="1:53">
       <c r="A8" s="1">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D8">
-        <v>35.30909</v>
+        <v>35.016491</v>
       </c>
       <c r="E8">
-        <v>-85.14274</v>
+        <v>-85.28069000000001</v>
       </c>
       <c r="F8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H8" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="K8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="P8" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="Y8">
         <v>4</v>
@@ -1097,31 +1076,31 @@
     </row>
     <row r="9" spans="1:53">
       <c r="A9" s="1">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
         <v>52</v>
       </c>
       <c r="D9">
-        <v>35.137319</v>
+        <v>35.016491</v>
       </c>
       <c r="E9">
-        <v>-85.23677000000001</v>
+        <v>-85.28069000000001</v>
       </c>
       <c r="F9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H9" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="K9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="P9" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="Y9">
         <v>4</v>
@@ -1129,31 +1108,31 @@
     </row>
     <row r="10" spans="1:53">
       <c r="A10" s="1">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
         <v>52</v>
       </c>
       <c r="D10">
-        <v>35.003256</v>
+        <v>35.015381</v>
       </c>
       <c r="E10">
-        <v>-85.28007700000001</v>
+        <v>-85.276945</v>
       </c>
       <c r="F10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H10" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="K10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="P10" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="Y10">
         <v>4</v>
@@ -1161,31 +1140,31 @@
     </row>
     <row r="11" spans="1:53">
       <c r="A11" s="1">
-        <v>92</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
         <v>52</v>
       </c>
       <c r="D11">
-        <v>35.035012</v>
+        <v>35.015381</v>
       </c>
       <c r="E11">
-        <v>-85.303878</v>
+        <v>-85.276945</v>
       </c>
       <c r="F11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H11" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="K11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="P11" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="Y11">
         <v>4</v>
@@ -1193,31 +1172,31 @@
     </row>
     <row r="12" spans="1:53">
       <c r="A12" s="1">
-        <v>93</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D12">
-        <v>35.035012</v>
+        <v>35.04156</v>
       </c>
       <c r="E12">
-        <v>-85.303878</v>
+        <v>-85.154814</v>
       </c>
       <c r="F12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G12" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H12" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="K12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="P12" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="Y12">
         <v>4</v>
@@ -1225,31 +1204,31 @@
     </row>
     <row r="13" spans="1:53">
       <c r="A13" s="1">
-        <v>105</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
         <v>53</v>
       </c>
       <c r="D13">
-        <v>35.041303</v>
+        <v>35.04156</v>
       </c>
       <c r="E13">
-        <v>-85.153824</v>
+        <v>-85.154814</v>
       </c>
       <c r="F13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G13" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H13" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="K13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="P13" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="Y13">
         <v>4</v>
@@ -1257,31 +1236,31 @@
     </row>
     <row r="14" spans="1:53">
       <c r="A14" s="1">
-        <v>111</v>
+        <v>50</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D14">
-        <v>34.996081</v>
+        <v>34.998805</v>
       </c>
       <c r="E14">
-        <v>-85.206737</v>
+        <v>-85.314233</v>
       </c>
       <c r="F14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G14" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H14" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="K14" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="P14" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="Y14">
         <v>4</v>
@@ -1289,31 +1268,31 @@
     </row>
     <row r="15" spans="1:53">
       <c r="A15" s="1">
-        <v>111</v>
+        <v>54</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D15">
-        <v>34.996081</v>
+        <v>35.069722</v>
       </c>
       <c r="E15">
-        <v>-85.206737</v>
+        <v>-85.100611</v>
       </c>
       <c r="F15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H15" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="K15" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="P15" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="Y15">
         <v>4</v>
@@ -1321,31 +1300,31 @@
     </row>
     <row r="16" spans="1:53">
       <c r="A16" s="1">
-        <v>116</v>
+        <v>56</v>
       </c>
       <c r="C16" t="s">
         <v>52</v>
       </c>
       <c r="D16">
-        <v>35.030596</v>
+        <v>35.21406</v>
       </c>
       <c r="E16">
-        <v>-85.362297</v>
+        <v>-85.21698000000001</v>
       </c>
       <c r="F16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H16" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="K16" t="s">
         <v>97</v>
       </c>
       <c r="P16" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="Y16">
         <v>4</v>
@@ -1353,31 +1332,31 @@
     </row>
     <row r="17" spans="1:25">
       <c r="A17" s="1">
-        <v>117</v>
+        <v>60</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D17">
-        <v>35.020581</v>
+        <v>35.190361</v>
       </c>
       <c r="E17">
-        <v>-85.36582</v>
+        <v>-85.24278</v>
       </c>
       <c r="F17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H17" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="K17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="P17" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="Y17">
         <v>4</v>
@@ -1385,31 +1364,31 @@
     </row>
     <row r="18" spans="1:25">
       <c r="A18" s="1">
-        <v>118</v>
+        <v>76</v>
       </c>
       <c r="C18" t="s">
         <v>52</v>
       </c>
       <c r="D18">
-        <v>35.020581</v>
+        <v>35.086481</v>
       </c>
       <c r="E18">
-        <v>-85.36582</v>
+        <v>-85.069652</v>
       </c>
       <c r="F18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H18" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="K18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="P18" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="Y18">
         <v>4</v>
@@ -1417,31 +1396,31 @@
     </row>
     <row r="19" spans="1:25">
       <c r="A19" s="1">
-        <v>125</v>
+        <v>77</v>
       </c>
       <c r="C19" t="s">
         <v>52</v>
       </c>
       <c r="D19">
-        <v>34.995549</v>
+        <v>35.086481</v>
       </c>
       <c r="E19">
-        <v>-85.20746800000001</v>
+        <v>-85.069652</v>
       </c>
       <c r="F19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G19" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H19" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="K19" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="P19" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="Y19">
         <v>4</v>
@@ -1449,31 +1428,31 @@
     </row>
     <row r="20" spans="1:25">
       <c r="A20" s="1">
-        <v>128</v>
+        <v>88</v>
       </c>
       <c r="C20" t="s">
         <v>52</v>
       </c>
       <c r="D20">
-        <v>35.062628</v>
+        <v>35.020273</v>
       </c>
       <c r="E20">
-        <v>-85.194113</v>
+        <v>-85.16169600000001</v>
       </c>
       <c r="F20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G20" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H20" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="K20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="P20" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="Y20">
         <v>4</v>
@@ -1481,31 +1460,31 @@
     </row>
     <row r="21" spans="1:25">
       <c r="A21" s="1">
-        <v>129</v>
+        <v>92</v>
       </c>
       <c r="C21" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D21">
-        <v>35.062628</v>
+        <v>35.132877</v>
       </c>
       <c r="E21">
-        <v>-85.194113</v>
+        <v>-85.23830700000001</v>
       </c>
       <c r="F21" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G21" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H21" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="K21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="P21" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="Y21">
         <v>4</v>
@@ -1513,31 +1492,31 @@
     </row>
     <row r="22" spans="1:25">
       <c r="A22" s="1">
-        <v>130</v>
+        <v>94</v>
       </c>
       <c r="C22" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D22">
-        <v>35.062628</v>
+        <v>35.01318</v>
       </c>
       <c r="E22">
-        <v>-85.194113</v>
+        <v>-85.228784</v>
       </c>
       <c r="F22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G22" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H22" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="P22" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="Y22">
         <v>4</v>
@@ -1545,65 +1524,33 @@
     </row>
     <row r="23" spans="1:25">
       <c r="A23" s="1">
-        <v>140</v>
+        <v>96</v>
       </c>
       <c r="C23" t="s">
         <v>52</v>
       </c>
       <c r="D23">
-        <v>35.072824</v>
+        <v>35.013646</v>
       </c>
       <c r="E23">
-        <v>-85.12366</v>
+        <v>-85.228888</v>
       </c>
       <c r="F23" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G23" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H23" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="K23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="P23" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="Y23">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:25">
-      <c r="A24" s="1">
-        <v>147</v>
-      </c>
-      <c r="C24" t="s">
-        <v>53</v>
-      </c>
-      <c r="D24">
-        <v>35.015818</v>
-      </c>
-      <c r="E24">
-        <v>-85.254192</v>
-      </c>
-      <c r="F24" t="s">
-        <v>56</v>
-      </c>
-      <c r="G24" t="s">
-        <v>78</v>
-      </c>
-      <c r="H24" t="s">
-        <v>96</v>
-      </c>
-      <c r="K24" t="s">
-        <v>100</v>
-      </c>
-      <c r="P24" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y24">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Made new file to hold grid stuff
</commit_message>
<xml_diff>
--- a/Excel & CSV Sheets/2019 Data/DailyReports/ToRemoveFile.xlsx
+++ b/Excel & CSV Sheets/2019 Data/DailyReports/ToRemoveFile.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="97">
   <si>
     <t>Accident</t>
   </si>
@@ -178,106 +178,118 @@
     <t>No Injuries</t>
   </si>
   <si>
-    <t>2019-05-09</t>
-  </si>
-  <si>
-    <t>21:27:04</t>
-  </si>
-  <si>
-    <t>16:17:15</t>
-  </si>
-  <si>
-    <t>16:16:52</t>
-  </si>
-  <si>
-    <t>16:10:26</t>
-  </si>
-  <si>
-    <t>16:01:45</t>
-  </si>
-  <si>
-    <t>16:01:17</t>
-  </si>
-  <si>
-    <t>15:51:07</t>
-  </si>
-  <si>
-    <t>15:48:43</t>
-  </si>
-  <si>
-    <t>13:08:23</t>
-  </si>
-  <si>
-    <t>13:07:47</t>
-  </si>
-  <si>
-    <t>12:57:40</t>
-  </si>
-  <si>
-    <t>12:57:30</t>
-  </si>
-  <si>
-    <t>11:41:20</t>
-  </si>
-  <si>
-    <t>09:38:04</t>
-  </si>
-  <si>
-    <t>09:09:30</t>
-  </si>
-  <si>
-    <t>08:42:28</t>
-  </si>
-  <si>
-    <t>1360 INTERSTATE 75 SB</t>
-  </si>
-  <si>
-    <t>256-269 Sequoyah Rd</t>
-  </si>
-  <si>
-    <t>3219 BROAD ST</t>
-  </si>
-  <si>
-    <t>Airpark Dr / Vance Rd</t>
-  </si>
-  <si>
-    <t>6501 Ramsey Rd</t>
-  </si>
-  <si>
-    <t>4208 N Access Rd</t>
-  </si>
-  <si>
-    <t>15113-15199 Dayton Pike</t>
-  </si>
-  <si>
-    <t>Mccallie Ave / Lindsay St</t>
-  </si>
-  <si>
-    <t>5900 Highway 58</t>
-  </si>
-  <si>
-    <t>100 Ochs Hwy</t>
-  </si>
-  <si>
-    <t>501-513 Council Fire Dr</t>
+    <t>Entrapment</t>
+  </si>
+  <si>
+    <t>2019-05-11</t>
+  </si>
+  <si>
+    <t>22:17:30</t>
+  </si>
+  <si>
+    <t>22:17:17</t>
+  </si>
+  <si>
+    <t>22:16:49</t>
+  </si>
+  <si>
+    <t>22:16:11</t>
+  </si>
+  <si>
+    <t>21:24:12</t>
+  </si>
+  <si>
+    <t>21:23:18</t>
+  </si>
+  <si>
+    <t>21:06:39</t>
+  </si>
+  <si>
+    <t>20:19:49</t>
+  </si>
+  <si>
+    <t>20:17:54</t>
+  </si>
+  <si>
+    <t>17:35:32</t>
+  </si>
+  <si>
+    <t>14:01:58</t>
+  </si>
+  <si>
+    <t>13:11:40</t>
+  </si>
+  <si>
+    <t>12:53:27</t>
+  </si>
+  <si>
+    <t>10:22:34</t>
+  </si>
+  <si>
+    <t>10:19:26</t>
+  </si>
+  <si>
+    <t>08:50:21</t>
+  </si>
+  <si>
+    <t>07:12:37</t>
+  </si>
+  <si>
+    <t>4300-4399 Bonny Oaks Dr</t>
+  </si>
+  <si>
+    <t>310 Greenway View Dr</t>
+  </si>
+  <si>
+    <t>1113-1199 Fernway Rd</t>
+  </si>
+  <si>
+    <t>Brainerd Rd / Sequoia Dr</t>
+  </si>
+  <si>
+    <t>10 - 19 Exit 178 S Off Ramp Eb</t>
+  </si>
+  <si>
+    <t>7020 SHALLOWFORD RD</t>
+  </si>
+  <si>
+    <t>Belvoir Ave / S Terrace</t>
+  </si>
+  <si>
+    <t>2501 CUMMINGS HWY</t>
+  </si>
+  <si>
+    <t>6500 Lee Hwy</t>
+  </si>
+  <si>
+    <t>1-9 Exit 4 Off Ramp Sb</t>
+  </si>
+  <si>
+    <t>950 INTERSTATE 75 SB</t>
+  </si>
+  <si>
+    <t>5850-5957 Hunter Rd</t>
+  </si>
+  <si>
+    <t>CHATTANOOGA</t>
   </si>
   <si>
     <t>HAMILTON COUNTY</t>
   </si>
   <si>
-    <t>SODDY DAISY</t>
-  </si>
-  <si>
-    <t>CHATTANOOGA</t>
+    <t>22</t>
   </si>
   <si>
     <t>21</t>
   </si>
   <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>15</t>
+    <t>20</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>14</t>
   </si>
   <si>
     <t>13</t>
@@ -286,13 +298,13 @@
     <t>12</t>
   </si>
   <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>9</t>
+    <t>10</t>
   </si>
   <si>
     <t>8</t>
+  </si>
+  <si>
+    <t>7</t>
   </si>
 </sst>
 </file>
@@ -650,7 +662,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BA18"/>
+  <dimension ref="A1:BA20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -816,31 +828,31 @@
     </row>
     <row r="2" spans="1:53">
       <c r="A2" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
         <v>52</v>
       </c>
       <c r="D2">
-        <v>35.109425</v>
+        <v>35.08137</v>
       </c>
       <c r="E2">
-        <v>-85.04991699999999</v>
+        <v>-85.209672</v>
       </c>
       <c r="F2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="P2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="Y2">
         <v>5</v>
@@ -848,31 +860,31 @@
     </row>
     <row r="3" spans="1:53">
       <c r="A3" s="1">
-        <v>41</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
         <v>52</v>
       </c>
       <c r="D3">
-        <v>35.248455</v>
+        <v>35.08137</v>
       </c>
       <c r="E3">
-        <v>-85.17887500000001</v>
+        <v>-85.209672</v>
       </c>
       <c r="F3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="P3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="Y3">
         <v>5</v>
@@ -880,31 +892,31 @@
     </row>
     <row r="4" spans="1:53">
       <c r="A4" s="1">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
         <v>52</v>
       </c>
       <c r="D4">
-        <v>35.248455</v>
+        <v>35.01056</v>
       </c>
       <c r="E4">
-        <v>-85.17887500000001</v>
+        <v>-85.20740000000001</v>
       </c>
       <c r="F4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="K4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="P4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="Y4">
         <v>5</v>
@@ -912,31 +924,31 @@
     </row>
     <row r="5" spans="1:53">
       <c r="A5" s="1">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
         <v>52</v>
       </c>
       <c r="D5">
-        <v>35.018125</v>
+        <v>35.01056</v>
       </c>
       <c r="E5">
-        <v>-85.32198</v>
+        <v>-85.20740000000001</v>
       </c>
       <c r="F5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="P5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="Y5">
         <v>5</v>
@@ -944,31 +956,31 @@
     </row>
     <row r="6" spans="1:53">
       <c r="A6" s="1">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
         <v>52</v>
       </c>
       <c r="D6">
-        <v>35.034104</v>
+        <v>35.08476</v>
       </c>
       <c r="E6">
-        <v>-85.186956</v>
+        <v>-85.29191</v>
       </c>
       <c r="F6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="K6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="P6" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="Y6">
         <v>5</v>
@@ -976,31 +988,31 @@
     </row>
     <row r="7" spans="1:53">
       <c r="A7" s="1">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D7">
-        <v>35.034104</v>
+        <v>35.08477</v>
       </c>
       <c r="E7">
-        <v>-85.186956</v>
+        <v>-85.29192999999999</v>
       </c>
       <c r="F7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="K7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="P7" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="Y7">
         <v>5</v>
@@ -1008,19 +1020,19 @@
     </row>
     <row r="8" spans="1:53">
       <c r="A8" s="1">
-        <v>58</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D8">
-        <v>35.16791</v>
+        <v>35.08477</v>
       </c>
       <c r="E8">
-        <v>-85.099041</v>
+        <v>-85.29192999999999</v>
       </c>
       <c r="F8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G8" t="s">
         <v>61</v>
@@ -1029,10 +1041,10 @@
         <v>75</v>
       </c>
       <c r="K8" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="P8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="Y8">
         <v>5</v>
@@ -1040,31 +1052,31 @@
     </row>
     <row r="9" spans="1:53">
       <c r="A9" s="1">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
         <v>52</v>
       </c>
       <c r="D9">
-        <v>35.16791</v>
+        <v>35.015339</v>
       </c>
       <c r="E9">
-        <v>-85.099041</v>
+        <v>-85.233935</v>
       </c>
       <c r="F9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G9" t="s">
         <v>62</v>
       </c>
       <c r="H9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K9" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="P9" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="Y9">
         <v>5</v>
@@ -1072,31 +1084,31 @@
     </row>
     <row r="10" spans="1:53">
       <c r="A10" s="1">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
         <v>52</v>
       </c>
       <c r="D10">
-        <v>35.112875</v>
+        <v>35.03111</v>
       </c>
       <c r="E10">
-        <v>-85.255402</v>
+        <v>-85.320446</v>
       </c>
       <c r="F10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G10" t="s">
         <v>63</v>
       </c>
       <c r="H10" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="K10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="P10" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="Y10">
         <v>5</v>
@@ -1104,31 +1116,31 @@
     </row>
     <row r="11" spans="1:53">
       <c r="A11" s="1">
-        <v>79</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
         <v>52</v>
       </c>
       <c r="D11">
-        <v>35.112875</v>
+        <v>35.03111</v>
       </c>
       <c r="E11">
-        <v>-85.255402</v>
+        <v>-85.320446</v>
       </c>
       <c r="F11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G11" t="s">
         <v>64</v>
       </c>
       <c r="H11" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="K11" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="P11" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="Y11">
         <v>5</v>
@@ -1136,31 +1148,31 @@
     </row>
     <row r="12" spans="1:53">
       <c r="A12" s="1">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
         <v>52</v>
       </c>
       <c r="D12">
-        <v>35.384953</v>
+        <v>35.043326</v>
       </c>
       <c r="E12">
-        <v>-85.10852300000001</v>
+        <v>-85.15811100000001</v>
       </c>
       <c r="F12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G12" t="s">
         <v>65</v>
       </c>
       <c r="H12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K12" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="P12" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="Y12">
         <v>5</v>
@@ -1168,31 +1180,31 @@
     </row>
     <row r="13" spans="1:53">
       <c r="A13" s="1">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D13">
-        <v>35.384953</v>
+        <v>35.01068</v>
       </c>
       <c r="E13">
-        <v>-85.10852300000001</v>
+        <v>-85.24405899999999</v>
       </c>
       <c r="F13" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G13" t="s">
         <v>66</v>
       </c>
       <c r="H13" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="K13" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="P13" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="Y13">
         <v>5</v>
@@ -1200,31 +1212,31 @@
     </row>
     <row r="14" spans="1:53">
       <c r="A14" s="1">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D14">
-        <v>35.047433</v>
+        <v>35.019963</v>
       </c>
       <c r="E14">
-        <v>-85.305564</v>
+        <v>-85.350661</v>
       </c>
       <c r="F14" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G14" t="s">
         <v>67</v>
       </c>
       <c r="H14" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="P14" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="Y14">
         <v>5</v>
@@ -1232,31 +1244,31 @@
     </row>
     <row r="15" spans="1:53">
       <c r="A15" s="1">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="C15" t="s">
         <v>52</v>
       </c>
       <c r="D15">
-        <v>35.113478</v>
+        <v>35.034605</v>
       </c>
       <c r="E15">
-        <v>-85.129991</v>
+        <v>-85.177768</v>
       </c>
       <c r="F15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G15" t="s">
         <v>68</v>
       </c>
       <c r="H15" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="K15" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="P15" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="Y15">
         <v>5</v>
@@ -1264,31 +1276,31 @@
     </row>
     <row r="16" spans="1:53">
       <c r="A16" s="1">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="C16" t="s">
         <v>52</v>
       </c>
       <c r="D16">
-        <v>35.113478</v>
+        <v>35.030718</v>
       </c>
       <c r="E16">
-        <v>-85.129991</v>
+        <v>-85.169021</v>
       </c>
       <c r="F16" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G16" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H16" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="K16" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="P16" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="Y16">
         <v>5</v>
@@ -1302,25 +1314,25 @@
         <v>52</v>
       </c>
       <c r="D17">
-        <v>35.008047</v>
+        <v>35.030718</v>
       </c>
       <c r="E17">
-        <v>-85.328467</v>
+        <v>-85.169021</v>
       </c>
       <c r="F17" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G17" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H17" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="K17" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="P17" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="Y17">
         <v>5</v>
@@ -1328,33 +1340,97 @@
     </row>
     <row r="18" spans="1:25">
       <c r="A18" s="1">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C18" t="s">
         <v>52</v>
       </c>
       <c r="D18">
-        <v>34.98779</v>
+        <v>35.07634</v>
       </c>
       <c r="E18">
-        <v>-85.16379000000001</v>
+        <v>-85.10387799999999</v>
       </c>
       <c r="F18" t="s">
+        <v>55</v>
+      </c>
+      <c r="G18" t="s">
+        <v>71</v>
+      </c>
+      <c r="H18" t="s">
+        <v>83</v>
+      </c>
+      <c r="K18" t="s">
+        <v>85</v>
+      </c>
+      <c r="P18" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25">
+      <c r="A19" s="1">
+        <v>115</v>
+      </c>
+      <c r="C19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19">
+        <v>35.07634</v>
+      </c>
+      <c r="E19">
+        <v>-85.10387799999999</v>
+      </c>
+      <c r="F19" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" t="s">
+        <v>71</v>
+      </c>
+      <c r="H19" t="s">
+        <v>83</v>
+      </c>
+      <c r="K19" t="s">
+        <v>85</v>
+      </c>
+      <c r="P19" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25">
+      <c r="A20" s="1">
+        <v>125</v>
+      </c>
+      <c r="C20" t="s">
         <v>54</v>
       </c>
-      <c r="G18" t="s">
-        <v>70</v>
-      </c>
-      <c r="H18" t="s">
-        <v>81</v>
-      </c>
-      <c r="K18" t="s">
+      <c r="D20">
+        <v>35.121859</v>
+      </c>
+      <c r="E20">
+        <v>-85.08718</v>
+      </c>
+      <c r="F20" t="s">
+        <v>55</v>
+      </c>
+      <c r="G20" t="s">
+        <v>72</v>
+      </c>
+      <c r="H20" t="s">
         <v>84</v>
       </c>
-      <c r="P18" t="s">
-        <v>92</v>
-      </c>
-      <c r="Y18">
+      <c r="K20" t="s">
+        <v>86</v>
+      </c>
+      <c r="P20" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y20">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Completed First Forecast, have predictions
</commit_message>
<xml_diff>
--- a/Excel & CSV Sheets/2019 Data/DailyReports/ToRemoveFile.xlsx
+++ b/Excel & CSV Sheets/2019 Data/DailyReports/ToRemoveFile.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="76">
   <si>
     <t>Accident</t>
   </si>
@@ -178,127 +178,70 @@
     <t>No Injuries</t>
   </si>
   <si>
-    <t>Unknown Injuries</t>
-  </si>
-  <si>
-    <t>2019-05-13</t>
-  </si>
-  <si>
-    <t>20:12:57</t>
-  </si>
-  <si>
-    <t>20:11:39</t>
-  </si>
-  <si>
-    <t>18:22:50</t>
-  </si>
-  <si>
-    <t>14:16:44</t>
-  </si>
-  <si>
-    <t>13:51:22</t>
-  </si>
-  <si>
-    <t>13:05:06</t>
-  </si>
-  <si>
-    <t>13:04:12</t>
-  </si>
-  <si>
-    <t>09:04:15</t>
-  </si>
-  <si>
-    <t>09:03:23</t>
-  </si>
-  <si>
-    <t>09:02:13</t>
-  </si>
-  <si>
-    <t>08:43:36</t>
-  </si>
-  <si>
-    <t>08:42:13</t>
-  </si>
-  <si>
-    <t>08:05:36</t>
-  </si>
-  <si>
-    <t>07:37:08</t>
-  </si>
-  <si>
-    <t>07:35:24</t>
-  </si>
-  <si>
-    <t>00:42:43</t>
-  </si>
-  <si>
-    <t>1106 Green Pond Rd</t>
-  </si>
-  <si>
-    <t>Eveningside Dr / E Main St</t>
-  </si>
-  <si>
-    <t>6123 Mountain View Rd</t>
-  </si>
-  <si>
-    <t>100 Interstate 75 Nb</t>
-  </si>
-  <si>
-    <t>Standifer Gap Rd / Quail Run Dr</t>
-  </si>
-  <si>
-    <t>8700 QUAIL RUN DR</t>
-  </si>
-  <si>
-    <t>2000 Taft Hwy</t>
-  </si>
-  <si>
-    <t>1822 - 2199 Taft Hwy</t>
-  </si>
-  <si>
-    <t>6734 Lee Hwy</t>
-  </si>
-  <si>
-    <t>3346 Browndell Dr</t>
-  </si>
-  <si>
-    <t>1400 - 1807 Mowbray Pike</t>
+    <t>2019-05-14</t>
+  </si>
+  <si>
+    <t>23:15:58</t>
+  </si>
+  <si>
+    <t>23:15:57</t>
+  </si>
+  <si>
+    <t>23:15:35</t>
+  </si>
+  <si>
+    <t>20:28:28</t>
+  </si>
+  <si>
+    <t>16:13:15</t>
+  </si>
+  <si>
+    <t>07:34:29</t>
+  </si>
+  <si>
+    <t>07:32:53</t>
+  </si>
+  <si>
+    <t>07:12:32</t>
+  </si>
+  <si>
+    <t>N Orchard Knob Ave / E 3rd St</t>
+  </si>
+  <si>
+    <t>1900 E 3RD ST</t>
+  </si>
+  <si>
+    <t>7400 - 7469 Allemande Way</t>
+  </si>
+  <si>
+    <t>Thrasher Pike / Gann Rd</t>
+  </si>
+  <si>
+    <t>Kellys Ferry Rd / Browns Ferry Rd</t>
+  </si>
+  <si>
+    <t>176 - 199 Signal Mountain Rd</t>
+  </si>
+  <si>
+    <t>CHATTANOOGA</t>
   </si>
   <si>
     <t>SODDY DAISY</t>
   </si>
   <si>
-    <t>CHATTANOOGA</t>
-  </si>
-  <si>
-    <t>HAMILTON COUNTY</t>
-  </si>
-  <si>
-    <t>WALDEN</t>
+    <t>RED BANK</t>
+  </si>
+  <si>
+    <t>23</t>
   </si>
   <si>
     <t>20</t>
   </si>
   <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>8</t>
+    <t>16</t>
   </si>
   <si>
     <t>7</t>
-  </si>
-  <si>
-    <t>0</t>
   </si>
 </sst>
 </file>
@@ -656,7 +599,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BA17"/>
+  <dimension ref="A1:BA9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -822,31 +765,31 @@
     </row>
     <row r="2" spans="1:53">
       <c r="A2" s="1">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
         <v>52</v>
       </c>
       <c r="D2">
-        <v>35.238912</v>
+        <v>35.040879</v>
       </c>
       <c r="E2">
-        <v>-85.157837</v>
+        <v>-85.27199</v>
       </c>
       <c r="F2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" t="s">
         <v>55</v>
       </c>
-      <c r="G2" t="s">
-        <v>56</v>
-      </c>
       <c r="H2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K2" t="s">
+        <v>69</v>
+      </c>
+      <c r="P2" t="s">
         <v>72</v>
-      </c>
-      <c r="K2" t="s">
-        <v>83</v>
-      </c>
-      <c r="P2" t="s">
-        <v>87</v>
       </c>
       <c r="Y2">
         <v>5</v>
@@ -854,31 +797,31 @@
     </row>
     <row r="3" spans="1:53">
       <c r="A3" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
         <v>52</v>
       </c>
       <c r="D3">
-        <v>35.238912</v>
+        <v>35.040879</v>
       </c>
       <c r="E3">
-        <v>-85.157837</v>
+        <v>-85.27199</v>
       </c>
       <c r="F3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H3" t="s">
+        <v>63</v>
+      </c>
+      <c r="K3" t="s">
+        <v>69</v>
+      </c>
+      <c r="P3" t="s">
         <v>72</v>
-      </c>
-      <c r="K3" t="s">
-        <v>83</v>
-      </c>
-      <c r="P3" t="s">
-        <v>87</v>
       </c>
       <c r="Y3">
         <v>5</v>
@@ -886,31 +829,31 @@
     </row>
     <row r="4" spans="1:53">
       <c r="A4" s="1">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
         <v>52</v>
       </c>
       <c r="D4">
-        <v>35.027314</v>
+        <v>35.040879</v>
       </c>
       <c r="E4">
-        <v>-85.283592</v>
+        <v>-85.27199</v>
       </c>
       <c r="F4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H4" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="K4" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="P4" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="Y4">
         <v>5</v>
@@ -918,31 +861,31 @@
     </row>
     <row r="5" spans="1:53">
       <c r="A5" s="1">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D5">
-        <v>35.093487</v>
+        <v>35.049055</v>
       </c>
       <c r="E5">
-        <v>-85.06273</v>
+        <v>-85.144323</v>
       </c>
       <c r="F5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H5" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="K5" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="P5" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="Y5">
         <v>5</v>
@@ -950,28 +893,31 @@
     </row>
     <row r="6" spans="1:53">
       <c r="A6" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6">
+        <v>35.202555</v>
+      </c>
+      <c r="E6">
+        <v>-85.20743</v>
+      </c>
+      <c r="F6" t="s">
         <v>54</v>
       </c>
-      <c r="D6">
-        <v>34.996081</v>
-      </c>
-      <c r="E6">
-        <v>-85.206737</v>
-      </c>
-      <c r="F6" t="s">
-        <v>55</v>
-      </c>
       <c r="G6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H6" t="s">
-        <v>75</v>
+        <v>66</v>
+      </c>
+      <c r="K6" t="s">
+        <v>70</v>
       </c>
       <c r="P6" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="Y6">
         <v>5</v>
@@ -979,31 +925,31 @@
     </row>
     <row r="7" spans="1:53">
       <c r="A7" s="1">
-        <v>30</v>
+        <v>71</v>
       </c>
       <c r="C7" t="s">
         <v>52</v>
       </c>
       <c r="D7">
-        <v>35.027024</v>
+        <v>35.020581</v>
       </c>
       <c r="E7">
-        <v>-85.10110400000001</v>
+        <v>-85.36582</v>
       </c>
       <c r="F7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H7" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="K7" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="P7" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="Y7">
         <v>5</v>
@@ -1011,31 +957,31 @@
     </row>
     <row r="8" spans="1:53">
       <c r="A8" s="1">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="C8" t="s">
         <v>52</v>
       </c>
       <c r="D8">
-        <v>35.027024</v>
+        <v>35.020581</v>
       </c>
       <c r="E8">
-        <v>-85.10110400000001</v>
+        <v>-85.36582</v>
       </c>
       <c r="F8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H8" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="K8" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="P8" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="Y8">
         <v>5</v>
@@ -1043,286 +989,33 @@
     </row>
     <row r="9" spans="1:53">
       <c r="A9" s="1">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="C9" t="s">
         <v>52</v>
       </c>
       <c r="D9">
-        <v>35.154608</v>
+        <v>35.084709</v>
       </c>
       <c r="E9">
-        <v>-85.317162</v>
+        <v>-85.322991</v>
       </c>
       <c r="F9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H9" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="K9" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="P9" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="Y9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:53">
-      <c r="A10" s="1">
-        <v>45</v>
-      </c>
-      <c r="C10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D10">
-        <v>35.154608</v>
-      </c>
-      <c r="E10">
-        <v>-85.317162</v>
-      </c>
-      <c r="F10" t="s">
-        <v>55</v>
-      </c>
-      <c r="G10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H10" t="s">
-        <v>78</v>
-      </c>
-      <c r="K10" t="s">
-        <v>86</v>
-      </c>
-      <c r="P10" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:53">
-      <c r="A11" s="1">
-        <v>47</v>
-      </c>
-      <c r="C11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11">
-        <v>35.153111</v>
-      </c>
-      <c r="E11">
-        <v>-85.31934099999999</v>
-      </c>
-      <c r="F11" t="s">
-        <v>55</v>
-      </c>
-      <c r="G11" t="s">
-        <v>65</v>
-      </c>
-      <c r="H11" t="s">
-        <v>79</v>
-      </c>
-      <c r="K11" t="s">
-        <v>86</v>
-      </c>
-      <c r="P11" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:53">
-      <c r="A12" s="1">
-        <v>52</v>
-      </c>
-      <c r="C12" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12">
-        <v>35.038841</v>
-      </c>
-      <c r="E12">
-        <v>-85.171139</v>
-      </c>
-      <c r="F12" t="s">
-        <v>55</v>
-      </c>
-      <c r="G12" t="s">
-        <v>66</v>
-      </c>
-      <c r="H12" t="s">
-        <v>80</v>
-      </c>
-      <c r="K12" t="s">
-        <v>84</v>
-      </c>
-      <c r="P12" t="s">
-        <v>92</v>
-      </c>
-      <c r="Y12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:53">
-      <c r="A13" s="1">
-        <v>53</v>
-      </c>
-      <c r="C13" t="s">
-        <v>52</v>
-      </c>
-      <c r="D13">
-        <v>35.038841</v>
-      </c>
-      <c r="E13">
-        <v>-85.171139</v>
-      </c>
-      <c r="F13" t="s">
-        <v>55</v>
-      </c>
-      <c r="G13" t="s">
-        <v>67</v>
-      </c>
-      <c r="H13" t="s">
-        <v>80</v>
-      </c>
-      <c r="K13" t="s">
-        <v>84</v>
-      </c>
-      <c r="P13" t="s">
-        <v>92</v>
-      </c>
-      <c r="Y13">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:53">
-      <c r="A14" s="1">
-        <v>55</v>
-      </c>
-      <c r="C14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14">
-        <v>34.996081</v>
-      </c>
-      <c r="E14">
-        <v>-85.206737</v>
-      </c>
-      <c r="F14" t="s">
-        <v>55</v>
-      </c>
-      <c r="G14" t="s">
-        <v>68</v>
-      </c>
-      <c r="H14" t="s">
-        <v>75</v>
-      </c>
-      <c r="P14" t="s">
-        <v>92</v>
-      </c>
-      <c r="Y14">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:53">
-      <c r="A15" s="1">
-        <v>59</v>
-      </c>
-      <c r="C15" t="s">
-        <v>52</v>
-      </c>
-      <c r="D15">
-        <v>35.030034</v>
-      </c>
-      <c r="E15">
-        <v>-85.368026</v>
-      </c>
-      <c r="F15" t="s">
-        <v>55</v>
-      </c>
-      <c r="G15" t="s">
-        <v>69</v>
-      </c>
-      <c r="H15" t="s">
-        <v>81</v>
-      </c>
-      <c r="K15" t="s">
-        <v>84</v>
-      </c>
-      <c r="P15" t="s">
-        <v>93</v>
-      </c>
-      <c r="Y15">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:53">
-      <c r="A16" s="1">
-        <v>60</v>
-      </c>
-      <c r="C16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16">
-        <v>35.030034</v>
-      </c>
-      <c r="E16">
-        <v>-85.368026</v>
-      </c>
-      <c r="F16" t="s">
-        <v>55</v>
-      </c>
-      <c r="G16" t="s">
-        <v>70</v>
-      </c>
-      <c r="H16" t="s">
-        <v>81</v>
-      </c>
-      <c r="K16" t="s">
-        <v>84</v>
-      </c>
-      <c r="P16" t="s">
-        <v>93</v>
-      </c>
-      <c r="Y16">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:25">
-      <c r="A17" s="1">
-        <v>71</v>
-      </c>
-      <c r="C17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D17">
-        <v>35.265016</v>
-      </c>
-      <c r="E17">
-        <v>-85.21368200000001</v>
-      </c>
-      <c r="F17" t="s">
-        <v>55</v>
-      </c>
-      <c r="G17" t="s">
-        <v>71</v>
-      </c>
-      <c r="H17" t="s">
-        <v>82</v>
-      </c>
-      <c r="K17" t="s">
-        <v>85</v>
-      </c>
-      <c r="P17" t="s">
-        <v>94</v>
-      </c>
-      <c r="Y17">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Created new model with added variables
</commit_message>
<xml_diff>
--- a/Excel & CSV Sheets/2019 Data/DailyReports/ToRemoveFile.xlsx
+++ b/Excel & CSV Sheets/2019 Data/DailyReports/ToRemoveFile.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="101">
   <si>
     <t>Accident</t>
   </si>
@@ -172,121 +172,133 @@
     <t>Pavement_Type</t>
   </si>
   <si>
+    <t>Grid_Block</t>
+  </si>
+  <si>
     <t>Injuries</t>
   </si>
   <si>
-    <t>Entrapment</t>
-  </si>
-  <si>
     <t>No Injuries</t>
   </si>
   <si>
     <t>Unknown Injuries</t>
   </si>
   <si>
-    <t>2019-05-19</t>
-  </si>
-  <si>
-    <t>23:45:41</t>
-  </si>
-  <si>
-    <t>22:11:56</t>
-  </si>
-  <si>
-    <t>21:25:49</t>
-  </si>
-  <si>
-    <t>21:19:29</t>
-  </si>
-  <si>
-    <t>21:19:11</t>
-  </si>
-  <si>
-    <t>16:39:34</t>
-  </si>
-  <si>
-    <t>16:37:45</t>
-  </si>
-  <si>
-    <t>16:20:48</t>
-  </si>
-  <si>
-    <t>15:56:14</t>
-  </si>
-  <si>
-    <t>15:45:44</t>
-  </si>
-  <si>
-    <t>13:52:29</t>
-  </si>
-  <si>
-    <t>13:52:04</t>
-  </si>
-  <si>
-    <t>13:11:45</t>
-  </si>
-  <si>
-    <t>13:11:05</t>
-  </si>
-  <si>
-    <t>02:34:11</t>
-  </si>
-  <si>
-    <t>02:32:03</t>
-  </si>
-  <si>
-    <t>FRAWLEY RD / RINGGOLD RD</t>
-  </si>
-  <si>
-    <t>CENTRAL AVE / BAILEY AVE</t>
-  </si>
-  <si>
-    <t>6830 - 6879 E BRAINERD RD</t>
-  </si>
-  <si>
-    <t>900-998 Cherokee Blvd</t>
-  </si>
-  <si>
-    <t>17900 Interstate 24 Wb</t>
-  </si>
-  <si>
-    <t>600 HIGHWAY 153 NB</t>
-  </si>
-  <si>
-    <t>5724 Highway 153</t>
-  </si>
-  <si>
-    <t>10300 - 10699 Lee Hwy</t>
-  </si>
-  <si>
-    <t>50-119 Interstate 75 Nb</t>
-  </si>
-  <si>
-    <t>9800 LEE HWY</t>
-  </si>
-  <si>
-    <t>9800 - 10099 Lee Hwy</t>
-  </si>
-  <si>
-    <t>4513 Rogers Rd</t>
-  </si>
-  <si>
-    <t>EAST RIDGE</t>
+    <t>2019-05-22</t>
+  </si>
+  <si>
+    <t>20:50:03</t>
+  </si>
+  <si>
+    <t>20:49:30</t>
+  </si>
+  <si>
+    <t>18:51:50</t>
+  </si>
+  <si>
+    <t>17:40:10</t>
+  </si>
+  <si>
+    <t>17:21:07</t>
+  </si>
+  <si>
+    <t>16:56:57</t>
+  </si>
+  <si>
+    <t>16:42:14</t>
+  </si>
+  <si>
+    <t>16:41:17</t>
+  </si>
+  <si>
+    <t>16:11:09</t>
+  </si>
+  <si>
+    <t>15:40:29</t>
+  </si>
+  <si>
+    <t>12:24:22</t>
+  </si>
+  <si>
+    <t>12:20:56</t>
+  </si>
+  <si>
+    <t>12:18:19</t>
+  </si>
+  <si>
+    <t>10:37:56</t>
+  </si>
+  <si>
+    <t>10:36:25</t>
+  </si>
+  <si>
+    <t>10:30:04</t>
+  </si>
+  <si>
+    <t>08:12:09</t>
+  </si>
+  <si>
+    <t>07:27:18</t>
+  </si>
+  <si>
+    <t>8223 Old Lee Hwy</t>
+  </si>
+  <si>
+    <t>404 S Crest Rd</t>
+  </si>
+  <si>
+    <t>Williams St / W 16th St</t>
+  </si>
+  <si>
+    <t>400 - 499 W 33rd St</t>
+  </si>
+  <si>
+    <t>200 GEORGIA AVE</t>
+  </si>
+  <si>
+    <t>E 23rd St / Central Ave</t>
+  </si>
+  <si>
+    <t>3136 New York Ave</t>
+  </si>
+  <si>
+    <t>Dayton Blvd / E Midvale Ave</t>
+  </si>
+  <si>
+    <t>5518-5559 Highway 153</t>
+  </si>
+  <si>
+    <t>5110-5149 Highway 153</t>
+  </si>
+  <si>
+    <t>5110 Highway 153</t>
+  </si>
+  <si>
+    <t>518 - 599 Barton Ave</t>
+  </si>
+  <si>
+    <t>2133-2219 Hamill Rd</t>
+  </si>
+  <si>
+    <t>590 INTERSTATE 75 SB</t>
+  </si>
+  <si>
+    <t>170 INTERSTATE 75 SB</t>
   </si>
   <si>
     <t>CHATTANOOGA</t>
   </si>
   <si>
-    <t>COLLEGEDALE</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>21</t>
+    <t>RED BANK</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>17</t>
   </si>
   <si>
     <t>16</t>
@@ -295,10 +307,16 @@
     <t>15</t>
   </si>
   <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>2</t>
+    <t>12</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>7</t>
   </si>
 </sst>
 </file>
@@ -656,13 +674,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BA18"/>
+  <dimension ref="A1:BB21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:53">
+    <row r="1" spans="1:54">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -819,19 +837,22 @@
       <c r="BA1" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="2" spans="1:53">
+      <c r="BB1" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:54">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D2">
-        <v>34.988345</v>
+        <v>35.07167</v>
       </c>
       <c r="E2">
-        <v>-85.191565</v>
+        <v>-85.09801299999999</v>
       </c>
       <c r="F2" t="s">
         <v>56</v>
@@ -840,461 +861,461 @@
         <v>57</v>
       </c>
       <c r="H2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="K2" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="P2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="Y2">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:53">
+    <row r="3" spans="1:54">
       <c r="A3" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D3">
-        <v>35.039775</v>
+        <v>35.07167</v>
       </c>
       <c r="E3">
-        <v>-85.292119</v>
+        <v>-85.09801299999999</v>
       </c>
       <c r="F3" t="s">
         <v>56</v>
       </c>
       <c r="G3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H3" t="s">
+        <v>75</v>
+      </c>
+      <c r="K3" t="s">
+        <v>90</v>
+      </c>
+      <c r="P3" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:54">
+      <c r="A4" s="1">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4">
+        <v>35.07167</v>
+      </c>
+      <c r="E4">
+        <v>-85.09801299999999</v>
+      </c>
+      <c r="F4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" t="s">
         <v>58</v>
-      </c>
-      <c r="H3" t="s">
-        <v>74</v>
-      </c>
-      <c r="K3" t="s">
-        <v>86</v>
-      </c>
-      <c r="P3" t="s">
-        <v>89</v>
-      </c>
-      <c r="Y3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:53">
-      <c r="A4" s="1">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4">
-        <v>35.016889</v>
-      </c>
-      <c r="E4">
-        <v>-85.181912</v>
-      </c>
-      <c r="F4" t="s">
-        <v>56</v>
-      </c>
-      <c r="G4" t="s">
-        <v>59</v>
       </c>
       <c r="H4" t="s">
         <v>75</v>
       </c>
       <c r="K4" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="P4" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="Y4">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:53">
+    <row r="5" spans="1:54">
       <c r="A5" s="1">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D5">
-        <v>35.0733</v>
+        <v>35.005669</v>
       </c>
       <c r="E5">
-        <v>-85.31887999999999</v>
+        <v>-85.270718</v>
       </c>
       <c r="F5" t="s">
         <v>56</v>
       </c>
       <c r="G5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H5" t="s">
         <v>76</v>
       </c>
       <c r="K5" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="P5" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="Y5">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:53">
+    <row r="6" spans="1:54">
       <c r="A6" s="1">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D6">
-        <v>35.0733</v>
+        <v>35.036</v>
       </c>
       <c r="E6">
-        <v>-85.31887999999999</v>
+        <v>-85.309719</v>
       </c>
       <c r="F6" t="s">
         <v>56</v>
       </c>
       <c r="G6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="K6" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="P6" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="Y6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:53">
+    <row r="7" spans="1:54">
       <c r="A7" s="1">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D7">
-        <v>35.029438</v>
+        <v>35.036</v>
       </c>
       <c r="E7">
-        <v>-85.31139</v>
+        <v>-85.309719</v>
       </c>
       <c r="F7" t="s">
         <v>56</v>
       </c>
       <c r="G7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H7" t="s">
         <v>77</v>
       </c>
       <c r="K7" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="P7" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="Y7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:53">
+    <row r="8" spans="1:54">
       <c r="A8" s="1">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D8">
-        <v>35.029438</v>
+        <v>35.013401</v>
       </c>
       <c r="E8">
-        <v>-85.31139</v>
+        <v>-85.311116</v>
       </c>
       <c r="F8" t="s">
         <v>56</v>
       </c>
       <c r="G8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K8" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="P8" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="Y8">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:53">
+    <row r="9" spans="1:54">
       <c r="A9" s="1">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
         <v>54</v>
       </c>
       <c r="D9">
-        <v>35.094661</v>
+        <v>35.057563</v>
       </c>
       <c r="E9">
-        <v>-85.225106</v>
+        <v>-85.302503</v>
       </c>
       <c r="F9" t="s">
         <v>56</v>
       </c>
       <c r="G9" t="s">
+        <v>62</v>
+      </c>
+      <c r="H9" t="s">
+        <v>79</v>
+      </c>
+      <c r="K9" t="s">
+        <v>90</v>
+      </c>
+      <c r="P9" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:54">
+      <c r="A10" s="1">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10">
+        <v>35.024811</v>
+      </c>
+      <c r="E10">
+        <v>-85.299691</v>
+      </c>
+      <c r="F10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" t="s">
+        <v>63</v>
+      </c>
+      <c r="H10" t="s">
+        <v>80</v>
+      </c>
+      <c r="K10" t="s">
+        <v>90</v>
+      </c>
+      <c r="P10" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:54">
+      <c r="A11" s="1">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11">
+        <v>35.024811</v>
+      </c>
+      <c r="E11">
+        <v>-85.299691</v>
+      </c>
+      <c r="F11" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" t="s">
         <v>64</v>
-      </c>
-      <c r="H9" t="s">
-        <v>78</v>
-      </c>
-      <c r="K9" t="s">
-        <v>86</v>
-      </c>
-      <c r="P9" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:53">
-      <c r="A10" s="1">
-        <v>44</v>
-      </c>
-      <c r="C10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10">
-        <v>35.15336</v>
-      </c>
-      <c r="E10">
-        <v>-85.24834</v>
-      </c>
-      <c r="F10" t="s">
-        <v>56</v>
-      </c>
-      <c r="G10" t="s">
-        <v>65</v>
-      </c>
-      <c r="H10" t="s">
-        <v>79</v>
-      </c>
-      <c r="K10" t="s">
-        <v>86</v>
-      </c>
-      <c r="P10" t="s">
-        <v>92</v>
-      </c>
-      <c r="Y10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:53">
-      <c r="A11" s="1">
-        <v>49</v>
-      </c>
-      <c r="C11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11">
-        <v>35.084469</v>
-      </c>
-      <c r="E11">
-        <v>-85.024103</v>
-      </c>
-      <c r="F11" t="s">
-        <v>56</v>
-      </c>
-      <c r="G11" t="s">
-        <v>66</v>
       </c>
       <c r="H11" t="s">
         <v>80</v>
       </c>
       <c r="K11" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="P11" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="Y11">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:53">
+    <row r="12" spans="1:54">
       <c r="A12" s="1">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D12">
-        <v>34.999205</v>
+        <v>35.06847</v>
       </c>
       <c r="E12">
-        <v>-85.209816</v>
+        <v>-85.23316800000001</v>
       </c>
       <c r="F12" t="s">
         <v>56</v>
       </c>
       <c r="G12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H12" t="s">
         <v>81</v>
       </c>
       <c r="K12" t="s">
+        <v>90</v>
+      </c>
+      <c r="P12" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:54">
+      <c r="A13" s="1">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13">
+        <v>35.08929</v>
+      </c>
+      <c r="E13">
+        <v>-85.312495</v>
+      </c>
+      <c r="F13" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" t="s">
+        <v>66</v>
+      </c>
+      <c r="H13" t="s">
+        <v>82</v>
+      </c>
+      <c r="K13" t="s">
+        <v>91</v>
+      </c>
+      <c r="P13" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:54">
+      <c r="A14" s="1">
+        <v>51</v>
+      </c>
+      <c r="C14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14">
+        <v>35.145053</v>
+      </c>
+      <c r="E14">
+        <v>-85.249184</v>
+      </c>
+      <c r="F14" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" t="s">
+        <v>67</v>
+      </c>
+      <c r="H14" t="s">
+        <v>83</v>
+      </c>
+      <c r="K14" t="s">
+        <v>90</v>
+      </c>
+      <c r="P14" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:54">
+      <c r="A15" s="1">
+        <v>55</v>
+      </c>
+      <c r="C15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15">
+        <v>35.121571</v>
+      </c>
+      <c r="E15">
+        <v>-85.238322</v>
+      </c>
+      <c r="F15" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" t="s">
+        <v>68</v>
+      </c>
+      <c r="H15" t="s">
+        <v>84</v>
+      </c>
+      <c r="K15" t="s">
+        <v>90</v>
+      </c>
+      <c r="P15" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:54">
+      <c r="A16" s="1">
+        <v>56</v>
+      </c>
+      <c r="C16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16">
+        <v>35.12204</v>
+      </c>
+      <c r="E16">
+        <v>-85.238018</v>
+      </c>
+      <c r="F16" t="s">
+        <v>56</v>
+      </c>
+      <c r="G16" t="s">
+        <v>69</v>
+      </c>
+      <c r="H16" t="s">
         <v>85</v>
       </c>
-      <c r="P12" t="s">
-        <v>93</v>
-      </c>
-      <c r="Y12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:53">
-      <c r="A13" s="1">
-        <v>56</v>
-      </c>
-      <c r="C13" t="s">
-        <v>52</v>
-      </c>
-      <c r="D13">
-        <v>34.999205</v>
-      </c>
-      <c r="E13">
-        <v>-85.209816</v>
-      </c>
-      <c r="F13" t="s">
-        <v>56</v>
-      </c>
-      <c r="G13" t="s">
-        <v>68</v>
-      </c>
-      <c r="H13" t="s">
-        <v>81</v>
-      </c>
-      <c r="K13" t="s">
-        <v>85</v>
-      </c>
-      <c r="P13" t="s">
-        <v>93</v>
-      </c>
-      <c r="Y13">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:53">
-      <c r="A14" s="1">
-        <v>62</v>
-      </c>
-      <c r="C14" t="s">
-        <v>52</v>
-      </c>
-      <c r="D14">
-        <v>35.076678</v>
-      </c>
-      <c r="E14">
-        <v>-85.042866</v>
-      </c>
-      <c r="F14" t="s">
-        <v>56</v>
-      </c>
-      <c r="G14" t="s">
-        <v>69</v>
-      </c>
-      <c r="H14" t="s">
-        <v>82</v>
-      </c>
-      <c r="K14" t="s">
-        <v>87</v>
-      </c>
-      <c r="P14" t="s">
-        <v>93</v>
-      </c>
-      <c r="Y14">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:53">
-      <c r="A15" s="1">
-        <v>63</v>
-      </c>
-      <c r="C15" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15">
-        <v>35.076678</v>
-      </c>
-      <c r="E15">
-        <v>-85.042866</v>
-      </c>
-      <c r="F15" t="s">
-        <v>56</v>
-      </c>
-      <c r="G15" t="s">
-        <v>70</v>
-      </c>
-      <c r="H15" t="s">
-        <v>83</v>
-      </c>
-      <c r="K15" t="s">
-        <v>87</v>
-      </c>
-      <c r="P15" t="s">
-        <v>93</v>
-      </c>
-      <c r="Y15">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:53">
-      <c r="A16" s="1">
-        <v>63</v>
-      </c>
-      <c r="C16" t="s">
-        <v>55</v>
-      </c>
-      <c r="D16">
-        <v>35.076678</v>
-      </c>
-      <c r="E16">
-        <v>-85.042866</v>
-      </c>
-      <c r="F16" t="s">
-        <v>56</v>
-      </c>
-      <c r="G16" t="s">
-        <v>70</v>
-      </c>
-      <c r="H16" t="s">
-        <v>83</v>
-      </c>
       <c r="K16" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="P16" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="Y16">
         <v>5</v>
@@ -1302,31 +1323,31 @@
     </row>
     <row r="17" spans="1:25">
       <c r="A17" s="1">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="C17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D17">
-        <v>35.02529</v>
+        <v>35.064944</v>
       </c>
       <c r="E17">
-        <v>-85.22837</v>
+        <v>-85.295261</v>
       </c>
       <c r="F17" t="s">
         <v>56</v>
       </c>
       <c r="G17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H17" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="K17" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="P17" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="Y17">
         <v>5</v>
@@ -1334,33 +1355,129 @@
     </row>
     <row r="18" spans="1:25">
       <c r="A18" s="1">
+        <v>64</v>
+      </c>
+      <c r="C18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18">
+        <v>35.064944</v>
+      </c>
+      <c r="E18">
+        <v>-85.295261</v>
+      </c>
+      <c r="F18" t="s">
+        <v>56</v>
+      </c>
+      <c r="G18" t="s">
+        <v>71</v>
+      </c>
+      <c r="H18" t="s">
         <v>86</v>
       </c>
-      <c r="C18" t="s">
-        <v>52</v>
-      </c>
-      <c r="D18">
-        <v>35.02529</v>
-      </c>
-      <c r="E18">
-        <v>-85.22837</v>
-      </c>
-      <c r="F18" t="s">
-        <v>56</v>
-      </c>
-      <c r="G18" t="s">
+      <c r="K18" t="s">
+        <v>90</v>
+      </c>
+      <c r="P18" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25">
+      <c r="A19" s="1">
+        <v>70</v>
+      </c>
+      <c r="C19" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19">
+        <v>35.124376</v>
+      </c>
+      <c r="E19">
+        <v>-85.233897</v>
+      </c>
+      <c r="F19" t="s">
+        <v>56</v>
+      </c>
+      <c r="G19" t="s">
         <v>72</v>
       </c>
-      <c r="H18" t="s">
-        <v>84</v>
-      </c>
-      <c r="K18" t="s">
-        <v>86</v>
-      </c>
-      <c r="P18" t="s">
-        <v>94</v>
-      </c>
-      <c r="Y18">
+      <c r="H19" t="s">
+        <v>87</v>
+      </c>
+      <c r="K19" t="s">
+        <v>90</v>
+      </c>
+      <c r="P19" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25">
+      <c r="A20" s="1">
+        <v>85</v>
+      </c>
+      <c r="C20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20">
+        <v>35.045852</v>
+      </c>
+      <c r="E20">
+        <v>-85.152462</v>
+      </c>
+      <c r="F20" t="s">
+        <v>56</v>
+      </c>
+      <c r="G20" t="s">
+        <v>73</v>
+      </c>
+      <c r="H20" t="s">
+        <v>88</v>
+      </c>
+      <c r="K20" t="s">
+        <v>90</v>
+      </c>
+      <c r="P20" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25">
+      <c r="A21" s="1">
+        <v>97</v>
+      </c>
+      <c r="C21" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21">
+        <v>35.006927</v>
+      </c>
+      <c r="E21">
+        <v>-85.205022</v>
+      </c>
+      <c r="F21" t="s">
+        <v>56</v>
+      </c>
+      <c r="G21" t="s">
+        <v>74</v>
+      </c>
+      <c r="H21" t="s">
+        <v>89</v>
+      </c>
+      <c r="K21" t="s">
+        <v>90</v>
+      </c>
+      <c r="P21" t="s">
+        <v>100</v>
+      </c>
+      <c r="Y21">
         <v>5</v>
       </c>
     </row>

</xml_diff>